<commit_message>
w - finished 2nd chapter
</commit_message>
<xml_diff>
--- a/LICENCJAT/confision_matrix_multiclass.xlsx
+++ b/LICENCJAT/confision_matrix_multiclass.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KarolG\Desktop\Math-project\LICENCJAT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA33F8C-7AEF-410E-A4F4-0C9524CC8C7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02B24BE9-F50A-441C-93F2-D077BFDBA6D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D38A347-B96C-4B76-85CD-9316D41376D5}"/>
   </bookViews>
@@ -56,12 +56,6 @@
     <t>TN</t>
   </si>
   <si>
-    <t>rzeczywistość</t>
-  </si>
-  <si>
-    <t>przewidywanie</t>
-  </si>
-  <si>
     <t>+</t>
   </si>
   <si>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t>fałszywie negatywny - FP</t>
+  </si>
+  <si>
+    <t>wartości przewidywane</t>
+  </si>
+  <si>
+    <t>wartości rzeczywiste</t>
   </si>
 </sst>
 </file>
@@ -208,37 +208,37 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -563,8 +563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B03D7D-F799-4A85-AE97-640F8E82B781}">
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,18 +599,18 @@
       <c r="A2" s="1"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
-      <c r="D2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
+      <c r="D2" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
       <c r="N2" s="1"/>
     </row>
     <row r="3" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
     <row r="4" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="17" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -663,16 +663,16 @@
       <c r="E4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -681,22 +681,22 @@
       <c r="C5" s="2">
         <v>1</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -705,22 +705,22 @@
       <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
+      <c r="F6" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -729,16 +729,16 @@
       <c r="C7" s="2">
         <v>3</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -747,16 +747,16 @@
       <c r="C8" s="2">
         <v>4</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -765,16 +765,16 @@
       <c r="C9" s="2">
         <v>5</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -783,16 +783,16 @@
       <c r="C10" s="2">
         <v>6</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -801,16 +801,16 @@
       <c r="C11" s="2">
         <v>7</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -819,16 +819,16 @@
       <c r="C12" s="2">
         <v>8</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
-      <c r="K12" s="6"/>
-      <c r="L12" s="6"/>
-      <c r="M12" s="6"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:22" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -837,16 +837,16 @@
       <c r="C13" s="2">
         <v>9</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="6"/>
-      <c r="M13" s="6"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
       <c r="N13" s="1"/>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -892,82 +892,82 @@
     </row>
     <row r="17" spans="15:22" x14ac:dyDescent="0.25">
       <c r="O17" s="1"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
+      <c r="P17" s="14"/>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
+      <c r="U17" s="11"/>
       <c r="V17" s="1"/>
     </row>
     <row r="18" spans="15:22" x14ac:dyDescent="0.25">
       <c r="O18" s="1"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="U18" s="13"/>
+      <c r="P18" s="14"/>
+      <c r="Q18" s="14"/>
+      <c r="R18" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="U18" s="9"/>
       <c r="V18" s="1"/>
     </row>
     <row r="19" spans="15:22" x14ac:dyDescent="0.25">
       <c r="O19" s="1"/>
-      <c r="P19" s="14" t="s">
+      <c r="P19" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q19" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="Q19" s="15" t="s">
+      <c r="R19" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="R19" s="16" t="s">
+      <c r="S19" s="12"/>
+      <c r="T19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="S19" s="16"/>
-      <c r="T19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="U19" s="6"/>
+      <c r="U19" s="13"/>
       <c r="V19" s="1"/>
     </row>
     <row r="20" spans="15:22" x14ac:dyDescent="0.25">
       <c r="O20" s="1"/>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="16"/>
-      <c r="S20" s="16"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
       <c r="V20" s="1"/>
     </row>
     <row r="21" spans="15:22" x14ac:dyDescent="0.25">
       <c r="O21" s="1"/>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="15" t="s">
+      <c r="P21" s="8"/>
+      <c r="Q21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="R21" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="S21" s="13"/>
+      <c r="T21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="R21" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="S21" s="6"/>
-      <c r="T21" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="U21" s="16"/>
+      <c r="U21" s="12"/>
       <c r="V21" s="1"/>
     </row>
     <row r="22" spans="15:22" x14ac:dyDescent="0.25">
       <c r="O22" s="1"/>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="6"/>
-      <c r="S22" s="6"/>
-      <c r="T22" s="16"/>
-      <c r="U22" s="16"/>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
       <c r="V22" s="1"/>
     </row>
     <row r="23" spans="15:22" x14ac:dyDescent="0.25">
@@ -991,6 +991,14 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="E6:E13"/>
+    <mergeCell ref="F5:M5"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="D2:M2"/>
+    <mergeCell ref="F6:M13"/>
+    <mergeCell ref="F4:M4"/>
+    <mergeCell ref="D6:D13"/>
+    <mergeCell ref="B2:C3"/>
     <mergeCell ref="P19:P22"/>
     <mergeCell ref="R18:S18"/>
     <mergeCell ref="Q19:Q20"/>
@@ -1002,14 +1010,6 @@
     <mergeCell ref="R21:S22"/>
     <mergeCell ref="T21:U22"/>
     <mergeCell ref="P17:Q18"/>
-    <mergeCell ref="E6:E13"/>
-    <mergeCell ref="F5:M5"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="D2:M2"/>
-    <mergeCell ref="F6:M13"/>
-    <mergeCell ref="F4:M4"/>
-    <mergeCell ref="D6:D13"/>
-    <mergeCell ref="B2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>